<commit_message>
edit: experiment related parameters
</commit_message>
<xml_diff>
--- a/Logbook.xlsx
+++ b/Logbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Experimental Data\Oh-hyeon Choung\P5_ShortProjects\TPD_priority_map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69D90ED-32AF-4A17-82DF-499ACB991756}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285C8CD8-18E7-424C-8F9C-91E489E30EB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25275" windowHeight="10320" tabRatio="711" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>Experimenter</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>002</t>
+  </si>
+  <si>
+    <t>003</t>
   </si>
 </sst>
 </file>
@@ -722,7 +725,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="V1" sqref="V1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,6 +851,9 @@
       <c r="E2" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F2" s="3">
+        <v>2</v>
+      </c>
       <c r="I2" s="22"/>
       <c r="J2" s="11"/>
       <c r="K2" s="12"/>
@@ -873,6 +879,9 @@
       <c r="E3" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="F3" s="3">
+        <v>5</v>
+      </c>
       <c r="I3" s="22"/>
       <c r="J3" s="11"/>
       <c r="K3" s="2"/>
@@ -889,6 +898,9 @@
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
+      <c r="B4" s="45" t="s">
+        <v>40</v>
+      </c>
       <c r="C4" s="19"/>
       <c r="D4" s="20"/>
       <c r="E4" s="3" t="s">

</xml_diff>